<commit_message>
trying to seed db with dummy projects and running into issue associating dummy accounts
</commit_message>
<xml_diff>
--- a/cabinets_app/Final_Project_Table_Data.xlsx
+++ b/cabinets_app/Final_Project_Table_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/GD/Coding/codefellows/401/final-project/cabinets_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E679B895-AD7E-5641-927C-0DC875026B28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{DD590E5D-30F1-5E41-B83C-22EFF031F634}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{F88FDB1C-3FF9-4905-B676-5439EA0E3782}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{F88FDB1C-3FF9-4905-B676-5439EA0E3782}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="8" r:id="rId1"/>
@@ -1046,8 +1046,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1246,8 +1246,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>